<commit_message>
fixed mistakes in cheatsheet
</commit_message>
<xml_diff>
--- a/cheatsheet.xlsx
+++ b/cheatsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="13830" windowHeight="7140"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="13830" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="cheatsheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>adresace buňky</t>
   </si>
@@ -59,9 +59,6 @@
     <t>worksheet.row_dimensions[no_row].height = height</t>
   </si>
   <si>
-    <t>worksheet.row_dimensions[letter_column].width = width</t>
-  </si>
-  <si>
     <t>písmeno sloupce podle čísla</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>rozdělení buněk</t>
   </si>
   <si>
-    <t>Tahák (openpyxl)</t>
-  </si>
-  <si>
     <t>výběr rozsahu</t>
   </si>
   <si>
@@ -510,9 +504,6 @@
     </r>
   </si>
   <si>
-    <t>letter = get_column_letter[no_column]</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">cell.number_format = </t>
     </r>
@@ -1464,17 +1455,87 @@
   </si>
   <si>
     <r>
-      <t>cell.fill = PatternFill(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF660099"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-      </rPr>
-      <t>bgColor</t>
+      <t>worksheet.merge_cells(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>'B3:D5'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>worksheet.unmerge_cells(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>'B3:D5'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>všechny buňky po řádcích</t>
+  </si>
+  <si>
+    <t>všechny buňky po sloupcích</t>
+  </si>
+  <si>
+    <t>worksheet.rows</t>
+  </si>
+  <si>
+    <t>worksheet.columns</t>
+  </si>
+  <si>
+    <t>worksheet.column_dimensions[letter_column].width = width</t>
+  </si>
+  <si>
+    <t>letter = get_column_letter(no_column)</t>
+  </si>
+  <si>
+    <r>
+      <t>cell.fill = PatternFill(f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF660099"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t>gColor</t>
     </r>
     <r>
       <rPr>
@@ -1550,68 +1611,19 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>worksheet.merge_cells(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF008080"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-      </rPr>
-      <t>'B3:D5'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>worksheet.unmerge_cells(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF008080"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-      </rPr>
-      <t>'B3:D5'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-        <charset val="238"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>všechny buňky po řádcích</t>
-  </si>
-  <si>
-    <t>všechny buňky po sloupcích</t>
-  </si>
-  <si>
-    <t>worksheet.rows</t>
-  </si>
-  <si>
-    <t>worksheet.columns</t>
+    <t>číslo posledního řádku</t>
+  </si>
+  <si>
+    <t>číslo posledního sloupce</t>
+  </si>
+  <si>
+    <t>worksheet_vypis.max_column</t>
+  </si>
+  <si>
+    <t>worksheet_vypis.max_row</t>
+  </si>
+  <si>
+    <t>Tahák pro knihovnu openpyxl</t>
   </si>
 </sst>
 </file>
@@ -1707,12 +1719,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -1727,6 +1733,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -2019,7 +2031,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -2032,341 +2044,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="2"/>
+      <c r="A1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="6" t="s">
+    <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6" t="s">
+    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="6" t="s">
+    <row r="10" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8" t="s">
+    <row r="11" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
+    <row r="14" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="8" t="s">
+    <row r="16" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="8" t="s">
+    <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="8" t="s">
+    <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8" t="s">
+    <row r="19" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="8" t="s">
+    <row r="31" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="32" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+      <c r="B37" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+      <c r="B38" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="7"/>
-    </row>
-    <row r="42" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="8" t="s">
+    <row r="51" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="8" t="s">
+    <row r="53" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A45:A48"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>